<commit_message>
only display office drivers
</commit_message>
<xml_diff>
--- a/Full Schedule Test.xlsx
+++ b/Full Schedule Test.xlsx
@@ -1817,7 +1817,11 @@
           <t>Elijah</t>
         </is>
       </c>
-      <c r="S25" t="inlineStr"/>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>Driver, Gray Van</t>
+        </is>
+      </c>
       <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
display meet without descriptor
</commit_message>
<xml_diff>
--- a/Full Schedule Test.xlsx
+++ b/Full Schedule Test.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y88"/>
+  <dimension ref="A1:Y124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -797,9 +797,8 @@
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
-          <t>M: 4:15 AM MEET COLLEGE (SOUTHWEST)
-IL: 5:00 AM AT IL OFFICE 
-FV: 4:45 AM BALLARD</t>
+          <t xml:space="preserve">M: 4:15 AM MEET COLLEGE (SOUTHWEST)
+IL: 5:00 AM AT IL OFFICE </t>
         </is>
       </c>
       <c r="K9" t="inlineStr"/>
@@ -3247,7 +3246,9 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>4:15 AM MEET SOUTH RACINE COURT (HWY 43 &amp; Y)</t>
+          <t>M: 4:15 AM MEET SOUTH RACINE COURT (HWY 43 &amp; Y)
+IL: 5:00 MEET AT IL OFFICE
+FV: 12:00 MEET</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
@@ -3872,7 +3873,12 @@
           <t>Ashley P</t>
         </is>
       </c>
-      <c r="G64" t="inlineStr"/>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Driver, 1/2
+Silver Van</t>
+        </is>
+      </c>
       <c r="H64" t="inlineStr"/>
       <c r="I64" t="inlineStr"/>
       <c r="J64" t="inlineStr">
@@ -4034,7 +4040,12 @@
           <t>Michael N</t>
         </is>
       </c>
-      <c r="G67" t="inlineStr"/>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Driver, 1/2
+Silver Van</t>
+        </is>
+      </c>
       <c r="H67" t="inlineStr"/>
       <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr">
@@ -4138,7 +4149,11 @@
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr"/>
-      <c r="F70" t="inlineStr"/>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>6:00 AM START</t>
+        </is>
+      </c>
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr"/>
       <c r="I70" t="inlineStr"/>
@@ -4186,7 +4201,11 @@
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr"/>
-      <c r="F71" t="inlineStr"/>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>DC5-ITEM LEVEL</t>
+        </is>
+      </c>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
       <c r="I71" t="inlineStr"/>
@@ -4229,7 +4248,11 @@
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr"/>
-      <c r="F72" t="inlineStr"/>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>AURORA OUTPATIENT RX #1300 WAUTOMA</t>
+        </is>
+      </c>
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr"/>
       <c r="I72" t="inlineStr"/>
@@ -4272,7 +4295,11 @@
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr"/>
-      <c r="F73" t="inlineStr"/>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>900 E DIVISION ST</t>
+        </is>
+      </c>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr"/>
       <c r="I73" t="inlineStr"/>
@@ -4307,7 +4334,11 @@
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr"/>
-      <c r="F74" t="inlineStr"/>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/JhUR6bvog6YmBrm48</t>
+        </is>
+      </c>
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr"/>
       <c r="I74" t="inlineStr"/>
@@ -4342,7 +4373,11 @@
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr"/>
-      <c r="F75" t="inlineStr"/>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>NEED SCANNER HOODS FOR THIS RX</t>
+        </is>
+      </c>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
       <c r="I75" t="inlineStr"/>
@@ -4419,9 +4454,22 @@
       <c r="B77" t="inlineStr"/>
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr"/>
-      <c r="F77" t="inlineStr"/>
-      <c r="G77" t="inlineStr"/>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Sarah</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>@ Store. Equip, 
+help at Pig after</t>
+        </is>
+      </c>
       <c r="H77" t="inlineStr"/>
       <c r="I77" t="inlineStr">
         <is>
@@ -4470,9 +4518,21 @@
       <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr"/>
-      <c r="F78" t="inlineStr"/>
-      <c r="G78" t="inlineStr"/>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Lori</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>@ Store. help at Pig after</t>
+        </is>
+      </c>
       <c r="H78" t="inlineStr"/>
       <c r="I78" t="inlineStr">
         <is>
@@ -4600,8 +4660,16 @@
       <c r="B81" t="inlineStr"/>
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr"/>
-      <c r="E81" t="inlineStr"/>
-      <c r="F81" t="inlineStr"/>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>7:00 AM START</t>
+        </is>
+      </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr"/>
       <c r="I81" t="inlineStr"/>
@@ -4641,7 +4709,11 @@
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr"/>
-      <c r="F82" t="inlineStr"/>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>DC5-FINANCIAL</t>
+        </is>
+      </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr"/>
       <c r="I82" t="inlineStr"/>
@@ -4694,7 +4766,11 @@
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="inlineStr"/>
-      <c r="F83" t="inlineStr"/>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>PIGGLY WIGGLY #311, WAUPACA</t>
+        </is>
+      </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr"/>
       <c r="I83" t="inlineStr"/>
@@ -4729,7 +4805,11 @@
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr"/>
-      <c r="F84" t="inlineStr"/>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>810 W FULTON</t>
+        </is>
+      </c>
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="inlineStr"/>
       <c r="I84" t="inlineStr"/>
@@ -4764,7 +4844,11 @@
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="inlineStr"/>
-      <c r="F85" t="inlineStr"/>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/vay5nnowsSN2</t>
+        </is>
+      </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr"/>
       <c r="I85" t="inlineStr"/>
@@ -4817,9 +4901,21 @@
       <c r="B87" t="inlineStr"/>
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr"/>
-      <c r="E87" t="inlineStr"/>
-      <c r="F87" t="inlineStr"/>
-      <c r="G87" t="inlineStr"/>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Jerry S</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>@ Store, Equip</t>
+        </is>
+      </c>
       <c r="H87" t="inlineStr"/>
       <c r="I87" t="inlineStr"/>
       <c r="J87" t="inlineStr"/>
@@ -4848,9 +4944,21 @@
       <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr"/>
-      <c r="E88" t="inlineStr"/>
-      <c r="F88" t="inlineStr"/>
-      <c r="G88" t="inlineStr"/>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Lori</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>@ Store, help after Aurora</t>
+        </is>
+      </c>
       <c r="H88" t="inlineStr"/>
       <c r="I88" t="inlineStr"/>
       <c r="J88" t="inlineStr"/>
@@ -4878,6 +4986,1220 @@
       <c r="X88" t="inlineStr"/>
       <c r="Y88" t="inlineStr"/>
     </row>
+    <row r="89">
+      <c r="A89" t="inlineStr"/>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr"/>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>3)</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Sarah</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>@ Store, help after Aurora</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr"/>
+      <c r="I89" t="inlineStr"/>
+      <c r="J89" t="inlineStr"/>
+      <c r="K89" t="inlineStr"/>
+      <c r="L89" t="inlineStr"/>
+      <c r="M89" t="inlineStr"/>
+      <c r="N89" t="inlineStr"/>
+      <c r="O89" t="inlineStr"/>
+      <c r="P89" t="inlineStr"/>
+      <c r="Q89" t="inlineStr"/>
+      <c r="R89" t="inlineStr"/>
+      <c r="S89" t="inlineStr"/>
+      <c r="T89" t="inlineStr"/>
+      <c r="U89" t="inlineStr"/>
+      <c r="V89" t="inlineStr"/>
+      <c r="W89" t="inlineStr"/>
+      <c r="X89" t="inlineStr"/>
+      <c r="Y89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr"/>
+      <c r="B90" t="inlineStr"/>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr"/>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>4)</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Heather</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr"/>
+      <c r="I90" t="inlineStr"/>
+      <c r="J90" t="inlineStr"/>
+      <c r="K90" t="inlineStr"/>
+      <c r="L90" t="inlineStr"/>
+      <c r="M90" t="inlineStr"/>
+      <c r="N90" t="inlineStr"/>
+      <c r="O90" t="inlineStr"/>
+      <c r="P90" t="inlineStr"/>
+      <c r="Q90" t="inlineStr"/>
+      <c r="R90" t="inlineStr"/>
+      <c r="S90" t="inlineStr"/>
+      <c r="T90" t="inlineStr"/>
+      <c r="U90" t="inlineStr"/>
+      <c r="V90" t="inlineStr"/>
+      <c r="W90" t="inlineStr"/>
+      <c r="X90" t="inlineStr"/>
+      <c r="Y90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr"/>
+      <c r="B91" t="inlineStr"/>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr"/>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>5)</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Katie</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>@ Store, work w/ Serena</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr"/>
+      <c r="I91" t="inlineStr"/>
+      <c r="J91" t="inlineStr"/>
+      <c r="K91" t="inlineStr"/>
+      <c r="L91" t="inlineStr"/>
+      <c r="M91" t="inlineStr"/>
+      <c r="N91" t="inlineStr"/>
+      <c r="O91" t="inlineStr"/>
+      <c r="P91" t="inlineStr"/>
+      <c r="Q91" t="inlineStr"/>
+      <c r="R91" t="inlineStr"/>
+      <c r="S91" t="inlineStr"/>
+      <c r="T91" t="inlineStr"/>
+      <c r="U91" t="inlineStr"/>
+      <c r="V91" t="inlineStr"/>
+      <c r="W91" t="inlineStr"/>
+      <c r="X91" t="inlineStr"/>
+      <c r="Y91" t="inlineStr"/>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr"/>
+      <c r="B92" t="inlineStr"/>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr"/>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>6)</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Kirsten</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr"/>
+      <c r="I92" t="inlineStr"/>
+      <c r="J92" t="inlineStr"/>
+      <c r="K92" t="inlineStr"/>
+      <c r="L92" t="inlineStr"/>
+      <c r="M92" t="inlineStr"/>
+      <c r="N92" t="inlineStr"/>
+      <c r="O92" t="inlineStr"/>
+      <c r="P92" t="inlineStr"/>
+      <c r="Q92" t="inlineStr"/>
+      <c r="R92" t="inlineStr"/>
+      <c r="S92" t="inlineStr"/>
+      <c r="T92" t="inlineStr"/>
+      <c r="U92" t="inlineStr"/>
+      <c r="V92" t="inlineStr"/>
+      <c r="W92" t="inlineStr"/>
+      <c r="X92" t="inlineStr"/>
+      <c r="Y92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr"/>
+      <c r="B93" t="inlineStr"/>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr"/>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>7)</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Marcia</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr"/>
+      <c r="I93" t="inlineStr"/>
+      <c r="J93" t="inlineStr"/>
+      <c r="K93" t="inlineStr"/>
+      <c r="L93" t="inlineStr"/>
+      <c r="M93" t="inlineStr"/>
+      <c r="N93" t="inlineStr"/>
+      <c r="O93" t="inlineStr"/>
+      <c r="P93" t="inlineStr"/>
+      <c r="Q93" t="inlineStr"/>
+      <c r="R93" t="inlineStr"/>
+      <c r="S93" t="inlineStr"/>
+      <c r="T93" t="inlineStr"/>
+      <c r="U93" t="inlineStr"/>
+      <c r="V93" t="inlineStr"/>
+      <c r="W93" t="inlineStr"/>
+      <c r="X93" t="inlineStr"/>
+      <c r="Y93" t="inlineStr"/>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr"/>
+      <c r="B94" t="inlineStr"/>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr"/>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>8)</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Michelle</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr"/>
+      <c r="I94" t="inlineStr"/>
+      <c r="J94" t="inlineStr"/>
+      <c r="K94" t="inlineStr"/>
+      <c r="L94" t="inlineStr"/>
+      <c r="M94" t="inlineStr"/>
+      <c r="N94" t="inlineStr"/>
+      <c r="O94" t="inlineStr"/>
+      <c r="P94" t="inlineStr"/>
+      <c r="Q94" t="inlineStr"/>
+      <c r="R94" t="inlineStr"/>
+      <c r="S94" t="inlineStr"/>
+      <c r="T94" t="inlineStr"/>
+      <c r="U94" t="inlineStr"/>
+      <c r="V94" t="inlineStr"/>
+      <c r="W94" t="inlineStr"/>
+      <c r="X94" t="inlineStr"/>
+      <c r="Y94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr"/>
+      <c r="B95" t="inlineStr"/>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr"/>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>9)</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Serena</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>@ Store, 1st Day, work w/ Katie</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr"/>
+      <c r="I95" t="inlineStr"/>
+      <c r="J95" t="inlineStr"/>
+      <c r="K95" t="inlineStr"/>
+      <c r="L95" t="inlineStr"/>
+      <c r="M95" t="inlineStr"/>
+      <c r="N95" t="inlineStr"/>
+      <c r="O95" t="inlineStr"/>
+      <c r="P95" t="inlineStr"/>
+      <c r="Q95" t="inlineStr"/>
+      <c r="R95" t="inlineStr"/>
+      <c r="S95" t="inlineStr"/>
+      <c r="T95" t="inlineStr"/>
+      <c r="U95" t="inlineStr"/>
+      <c r="V95" t="inlineStr"/>
+      <c r="W95" t="inlineStr"/>
+      <c r="X95" t="inlineStr"/>
+      <c r="Y95" t="inlineStr"/>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr"/>
+      <c r="B96" t="inlineStr"/>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr"/>
+      <c r="E96" t="inlineStr"/>
+      <c r="F96" t="inlineStr"/>
+      <c r="G96" t="inlineStr"/>
+      <c r="H96" t="inlineStr"/>
+      <c r="I96" t="inlineStr"/>
+      <c r="J96" t="inlineStr"/>
+      <c r="K96" t="inlineStr"/>
+      <c r="L96" t="inlineStr"/>
+      <c r="M96" t="inlineStr"/>
+      <c r="N96" t="inlineStr"/>
+      <c r="O96" t="inlineStr"/>
+      <c r="P96" t="inlineStr"/>
+      <c r="Q96" t="inlineStr"/>
+      <c r="R96" t="inlineStr"/>
+      <c r="S96" t="inlineStr"/>
+      <c r="T96" t="inlineStr"/>
+      <c r="U96" t="inlineStr"/>
+      <c r="V96" t="inlineStr"/>
+      <c r="W96" t="inlineStr"/>
+      <c r="X96" t="inlineStr"/>
+      <c r="Y96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr"/>
+      <c r="B97" t="inlineStr"/>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr"/>
+      <c r="E97" t="inlineStr"/>
+      <c r="F97" t="inlineStr"/>
+      <c r="G97" t="inlineStr"/>
+      <c r="H97" t="inlineStr"/>
+      <c r="I97" t="inlineStr"/>
+      <c r="J97" t="inlineStr"/>
+      <c r="K97" t="inlineStr"/>
+      <c r="L97" t="inlineStr"/>
+      <c r="M97" t="inlineStr"/>
+      <c r="N97" t="inlineStr"/>
+      <c r="O97" t="inlineStr"/>
+      <c r="P97" t="inlineStr"/>
+      <c r="Q97" t="inlineStr"/>
+      <c r="R97" t="inlineStr"/>
+      <c r="S97" t="inlineStr"/>
+      <c r="T97" t="inlineStr"/>
+      <c r="U97" t="inlineStr"/>
+      <c r="V97" t="inlineStr"/>
+      <c r="W97" t="inlineStr"/>
+      <c r="X97" t="inlineStr"/>
+      <c r="Y97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr"/>
+      <c r="B98" t="inlineStr"/>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr"/>
+      <c r="E98" t="inlineStr"/>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>6:30 AM START</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr"/>
+      <c r="H98" t="inlineStr"/>
+      <c r="I98" t="inlineStr"/>
+      <c r="J98" t="inlineStr"/>
+      <c r="K98" t="inlineStr"/>
+      <c r="L98" t="inlineStr"/>
+      <c r="M98" t="inlineStr"/>
+      <c r="N98" t="inlineStr"/>
+      <c r="O98" t="inlineStr"/>
+      <c r="P98" t="inlineStr"/>
+      <c r="Q98" t="inlineStr"/>
+      <c r="R98" t="inlineStr"/>
+      <c r="S98" t="inlineStr"/>
+      <c r="T98" t="inlineStr"/>
+      <c r="U98" t="inlineStr"/>
+      <c r="V98" t="inlineStr"/>
+      <c r="W98" t="inlineStr"/>
+      <c r="X98" t="inlineStr"/>
+      <c r="Y98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr"/>
+      <c r="B99" t="inlineStr"/>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr"/>
+      <c r="E99" t="inlineStr"/>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>DC5-ITEM LEVEL</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr"/>
+      <c r="H99" t="inlineStr"/>
+      <c r="I99" t="inlineStr"/>
+      <c r="J99" t="inlineStr"/>
+      <c r="K99" t="inlineStr"/>
+      <c r="L99" t="inlineStr"/>
+      <c r="M99" t="inlineStr"/>
+      <c r="N99" t="inlineStr"/>
+      <c r="O99" t="inlineStr"/>
+      <c r="P99" t="inlineStr"/>
+      <c r="Q99" t="inlineStr"/>
+      <c r="R99" t="inlineStr"/>
+      <c r="S99" t="inlineStr"/>
+      <c r="T99" t="inlineStr"/>
+      <c r="U99" t="inlineStr"/>
+      <c r="V99" t="inlineStr"/>
+      <c r="W99" t="inlineStr"/>
+      <c r="X99" t="inlineStr"/>
+      <c r="Y99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr"/>
+      <c r="B100" t="inlineStr"/>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="inlineStr"/>
+      <c r="E100" t="inlineStr"/>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>KELLEY #63, SUN PRAIRIE MOBIL</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr"/>
+      <c r="H100" t="inlineStr"/>
+      <c r="I100" t="inlineStr"/>
+      <c r="J100" t="inlineStr"/>
+      <c r="K100" t="inlineStr"/>
+      <c r="L100" t="inlineStr"/>
+      <c r="M100" t="inlineStr"/>
+      <c r="N100" t="inlineStr"/>
+      <c r="O100" t="inlineStr"/>
+      <c r="P100" t="inlineStr"/>
+      <c r="Q100" t="inlineStr"/>
+      <c r="R100" t="inlineStr"/>
+      <c r="S100" t="inlineStr"/>
+      <c r="T100" t="inlineStr"/>
+      <c r="U100" t="inlineStr"/>
+      <c r="V100" t="inlineStr"/>
+      <c r="W100" t="inlineStr"/>
+      <c r="X100" t="inlineStr"/>
+      <c r="Y100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr"/>
+      <c r="B101" t="inlineStr"/>
+      <c r="C101" t="inlineStr"/>
+      <c r="D101" t="inlineStr"/>
+      <c r="E101" t="inlineStr"/>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>1010 DAVISON DR</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr"/>
+      <c r="H101" t="inlineStr"/>
+      <c r="I101" t="inlineStr"/>
+      <c r="J101" t="inlineStr"/>
+      <c r="K101" t="inlineStr"/>
+      <c r="L101" t="inlineStr"/>
+      <c r="M101" t="inlineStr"/>
+      <c r="N101" t="inlineStr"/>
+      <c r="O101" t="inlineStr"/>
+      <c r="P101" t="inlineStr"/>
+      <c r="Q101" t="inlineStr"/>
+      <c r="R101" t="inlineStr"/>
+      <c r="S101" t="inlineStr"/>
+      <c r="T101" t="inlineStr"/>
+      <c r="U101" t="inlineStr"/>
+      <c r="V101" t="inlineStr"/>
+      <c r="W101" t="inlineStr"/>
+      <c r="X101" t="inlineStr"/>
+      <c r="Y101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr"/>
+      <c r="B102" t="inlineStr"/>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr"/>
+      <c r="E102" t="inlineStr"/>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/AcJV9qEV2xQ2</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr"/>
+      <c r="H102" t="inlineStr"/>
+      <c r="I102" t="inlineStr"/>
+      <c r="J102" t="inlineStr"/>
+      <c r="K102" t="inlineStr"/>
+      <c r="L102" t="inlineStr"/>
+      <c r="M102" t="inlineStr"/>
+      <c r="N102" t="inlineStr"/>
+      <c r="O102" t="inlineStr"/>
+      <c r="P102" t="inlineStr"/>
+      <c r="Q102" t="inlineStr"/>
+      <c r="R102" t="inlineStr"/>
+      <c r="S102" t="inlineStr"/>
+      <c r="T102" t="inlineStr"/>
+      <c r="U102" t="inlineStr"/>
+      <c r="V102" t="inlineStr"/>
+      <c r="W102" t="inlineStr"/>
+      <c r="X102" t="inlineStr"/>
+      <c r="Y102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr"/>
+      <c r="B103" t="inlineStr"/>
+      <c r="C103" t="inlineStr"/>
+      <c r="D103" t="inlineStr"/>
+      <c r="E103" t="inlineStr"/>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>*IL Meet is 5:15 am at IL Office</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr"/>
+      <c r="H103" t="inlineStr"/>
+      <c r="I103" t="inlineStr"/>
+      <c r="J103" t="inlineStr"/>
+      <c r="K103" t="inlineStr"/>
+      <c r="L103" t="inlineStr"/>
+      <c r="M103" t="inlineStr"/>
+      <c r="N103" t="inlineStr"/>
+      <c r="O103" t="inlineStr"/>
+      <c r="P103" t="inlineStr"/>
+      <c r="Q103" t="inlineStr"/>
+      <c r="R103" t="inlineStr"/>
+      <c r="S103" t="inlineStr"/>
+      <c r="T103" t="inlineStr"/>
+      <c r="U103" t="inlineStr"/>
+      <c r="V103" t="inlineStr"/>
+      <c r="W103" t="inlineStr"/>
+      <c r="X103" t="inlineStr"/>
+      <c r="Y103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr"/>
+      <c r="B104" t="inlineStr"/>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="inlineStr"/>
+      <c r="E104" t="inlineStr"/>
+      <c r="F104" t="inlineStr"/>
+      <c r="G104" t="inlineStr"/>
+      <c r="H104" t="inlineStr"/>
+      <c r="I104" t="inlineStr"/>
+      <c r="J104" t="inlineStr"/>
+      <c r="K104" t="inlineStr"/>
+      <c r="L104" t="inlineStr"/>
+      <c r="M104" t="inlineStr"/>
+      <c r="N104" t="inlineStr"/>
+      <c r="O104" t="inlineStr"/>
+      <c r="P104" t="inlineStr"/>
+      <c r="Q104" t="inlineStr"/>
+      <c r="R104" t="inlineStr"/>
+      <c r="S104" t="inlineStr"/>
+      <c r="T104" t="inlineStr"/>
+      <c r="U104" t="inlineStr"/>
+      <c r="V104" t="inlineStr"/>
+      <c r="W104" t="inlineStr"/>
+      <c r="X104" t="inlineStr"/>
+      <c r="Y104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr"/>
+      <c r="B105" t="inlineStr"/>
+      <c r="C105" t="inlineStr"/>
+      <c r="D105" t="inlineStr"/>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Qiana</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>@ Store,
+Camry, Equip</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr"/>
+      <c r="I105" t="inlineStr"/>
+      <c r="J105" t="inlineStr"/>
+      <c r="K105" t="inlineStr"/>
+      <c r="L105" t="inlineStr"/>
+      <c r="M105" t="inlineStr"/>
+      <c r="N105" t="inlineStr"/>
+      <c r="O105" t="inlineStr"/>
+      <c r="P105" t="inlineStr"/>
+      <c r="Q105" t="inlineStr"/>
+      <c r="R105" t="inlineStr"/>
+      <c r="S105" t="inlineStr"/>
+      <c r="T105" t="inlineStr"/>
+      <c r="U105" t="inlineStr"/>
+      <c r="V105" t="inlineStr"/>
+      <c r="W105" t="inlineStr"/>
+      <c r="X105" t="inlineStr"/>
+      <c r="Y105" t="inlineStr"/>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr"/>
+      <c r="B106" t="inlineStr"/>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="inlineStr"/>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Eva</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr"/>
+      <c r="H106" t="inlineStr"/>
+      <c r="I106" t="inlineStr"/>
+      <c r="J106" t="inlineStr"/>
+      <c r="K106" t="inlineStr"/>
+      <c r="L106" t="inlineStr"/>
+      <c r="M106" t="inlineStr"/>
+      <c r="N106" t="inlineStr"/>
+      <c r="O106" t="inlineStr"/>
+      <c r="P106" t="inlineStr"/>
+      <c r="Q106" t="inlineStr"/>
+      <c r="R106" t="inlineStr"/>
+      <c r="S106" t="inlineStr"/>
+      <c r="T106" t="inlineStr"/>
+      <c r="U106" t="inlineStr"/>
+      <c r="V106" t="inlineStr"/>
+      <c r="W106" t="inlineStr"/>
+      <c r="X106" t="inlineStr"/>
+      <c r="Y106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr"/>
+      <c r="B107" t="inlineStr"/>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="inlineStr"/>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>3)</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Evelin</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr"/>
+      <c r="H107" t="inlineStr"/>
+      <c r="I107" t="inlineStr"/>
+      <c r="J107" t="inlineStr"/>
+      <c r="K107" t="inlineStr"/>
+      <c r="L107" t="inlineStr"/>
+      <c r="M107" t="inlineStr"/>
+      <c r="N107" t="inlineStr"/>
+      <c r="O107" t="inlineStr"/>
+      <c r="P107" t="inlineStr"/>
+      <c r="Q107" t="inlineStr"/>
+      <c r="R107" t="inlineStr"/>
+      <c r="S107" t="inlineStr"/>
+      <c r="T107" t="inlineStr"/>
+      <c r="U107" t="inlineStr"/>
+      <c r="V107" t="inlineStr"/>
+      <c r="W107" t="inlineStr"/>
+      <c r="X107" t="inlineStr"/>
+      <c r="Y107" t="inlineStr"/>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr"/>
+      <c r="B108" t="inlineStr"/>
+      <c r="C108" t="inlineStr"/>
+      <c r="D108" t="inlineStr"/>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>4)</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>Josie</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr"/>
+      <c r="I108" t="inlineStr"/>
+      <c r="J108" t="inlineStr"/>
+      <c r="K108" t="inlineStr"/>
+      <c r="L108" t="inlineStr"/>
+      <c r="M108" t="inlineStr"/>
+      <c r="N108" t="inlineStr"/>
+      <c r="O108" t="inlineStr"/>
+      <c r="P108" t="inlineStr"/>
+      <c r="Q108" t="inlineStr"/>
+      <c r="R108" t="inlineStr"/>
+      <c r="S108" t="inlineStr"/>
+      <c r="T108" t="inlineStr"/>
+      <c r="U108" t="inlineStr"/>
+      <c r="V108" t="inlineStr"/>
+      <c r="W108" t="inlineStr"/>
+      <c r="X108" t="inlineStr"/>
+      <c r="Y108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr"/>
+      <c r="B109" t="inlineStr"/>
+      <c r="C109" t="inlineStr"/>
+      <c r="D109" t="inlineStr"/>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>5)</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>Nate</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>Driver, Optima</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr"/>
+      <c r="I109" t="inlineStr"/>
+      <c r="J109" t="inlineStr"/>
+      <c r="K109" t="inlineStr"/>
+      <c r="L109" t="inlineStr"/>
+      <c r="M109" t="inlineStr"/>
+      <c r="N109" t="inlineStr"/>
+      <c r="O109" t="inlineStr"/>
+      <c r="P109" t="inlineStr"/>
+      <c r="Q109" t="inlineStr"/>
+      <c r="R109" t="inlineStr"/>
+      <c r="S109" t="inlineStr"/>
+      <c r="T109" t="inlineStr"/>
+      <c r="U109" t="inlineStr"/>
+      <c r="V109" t="inlineStr"/>
+      <c r="W109" t="inlineStr"/>
+      <c r="X109" t="inlineStr"/>
+      <c r="Y109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr"/>
+      <c r="B110" t="inlineStr"/>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="inlineStr"/>
+      <c r="E110" t="inlineStr"/>
+      <c r="F110" t="inlineStr"/>
+      <c r="G110" t="inlineStr"/>
+      <c r="H110" t="inlineStr"/>
+      <c r="I110" t="inlineStr"/>
+      <c r="J110" t="inlineStr"/>
+      <c r="K110" t="inlineStr"/>
+      <c r="L110" t="inlineStr"/>
+      <c r="M110" t="inlineStr"/>
+      <c r="N110" t="inlineStr"/>
+      <c r="O110" t="inlineStr"/>
+      <c r="P110" t="inlineStr"/>
+      <c r="Q110" t="inlineStr"/>
+      <c r="R110" t="inlineStr"/>
+      <c r="S110" t="inlineStr"/>
+      <c r="T110" t="inlineStr"/>
+      <c r="U110" t="inlineStr"/>
+      <c r="V110" t="inlineStr"/>
+      <c r="W110" t="inlineStr"/>
+      <c r="X110" t="inlineStr"/>
+      <c r="Y110" t="inlineStr"/>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr"/>
+      <c r="B111" t="inlineStr"/>
+      <c r="C111" t="inlineStr"/>
+      <c r="D111" t="inlineStr"/>
+      <c r="E111" t="inlineStr"/>
+      <c r="F111" t="inlineStr"/>
+      <c r="G111" t="inlineStr"/>
+      <c r="H111" t="inlineStr"/>
+      <c r="I111" t="inlineStr"/>
+      <c r="J111" t="inlineStr"/>
+      <c r="K111" t="inlineStr"/>
+      <c r="L111" t="inlineStr"/>
+      <c r="M111" t="inlineStr"/>
+      <c r="N111" t="inlineStr"/>
+      <c r="O111" t="inlineStr"/>
+      <c r="P111" t="inlineStr"/>
+      <c r="Q111" t="inlineStr"/>
+      <c r="R111" t="inlineStr"/>
+      <c r="S111" t="inlineStr"/>
+      <c r="T111" t="inlineStr"/>
+      <c r="U111" t="inlineStr"/>
+      <c r="V111" t="inlineStr"/>
+      <c r="W111" t="inlineStr"/>
+      <c r="X111" t="inlineStr"/>
+      <c r="Y111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr"/>
+      <c r="B112" t="inlineStr"/>
+      <c r="C112" t="inlineStr"/>
+      <c r="D112" t="inlineStr"/>
+      <c r="E112" t="inlineStr"/>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>6:30 AM START</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr"/>
+      <c r="H112" t="inlineStr"/>
+      <c r="I112" t="inlineStr"/>
+      <c r="J112" t="inlineStr"/>
+      <c r="K112" t="inlineStr"/>
+      <c r="L112" t="inlineStr"/>
+      <c r="M112" t="inlineStr"/>
+      <c r="N112" t="inlineStr"/>
+      <c r="O112" t="inlineStr"/>
+      <c r="P112" t="inlineStr"/>
+      <c r="Q112" t="inlineStr"/>
+      <c r="R112" t="inlineStr"/>
+      <c r="S112" t="inlineStr"/>
+      <c r="T112" t="inlineStr"/>
+      <c r="U112" t="inlineStr"/>
+      <c r="V112" t="inlineStr"/>
+      <c r="W112" t="inlineStr"/>
+      <c r="X112" t="inlineStr"/>
+      <c r="Y112" t="inlineStr"/>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr"/>
+      <c r="B113" t="inlineStr"/>
+      <c r="C113" t="inlineStr"/>
+      <c r="D113" t="inlineStr"/>
+      <c r="E113" t="inlineStr"/>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>MODAS</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr"/>
+      <c r="H113" t="inlineStr"/>
+      <c r="I113" t="inlineStr"/>
+      <c r="J113" t="inlineStr"/>
+      <c r="K113" t="inlineStr"/>
+      <c r="L113" t="inlineStr"/>
+      <c r="M113" t="inlineStr"/>
+      <c r="N113" t="inlineStr"/>
+      <c r="O113" t="inlineStr"/>
+      <c r="P113" t="inlineStr"/>
+      <c r="Q113" t="inlineStr"/>
+      <c r="R113" t="inlineStr"/>
+      <c r="S113" t="inlineStr"/>
+      <c r="T113" t="inlineStr"/>
+      <c r="U113" t="inlineStr"/>
+      <c r="V113" t="inlineStr"/>
+      <c r="W113" t="inlineStr"/>
+      <c r="X113" t="inlineStr"/>
+      <c r="Y113" t="inlineStr"/>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr"/>
+      <c r="B114" t="inlineStr"/>
+      <c r="C114" t="inlineStr"/>
+      <c r="D114" t="inlineStr"/>
+      <c r="E114" t="inlineStr"/>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>KELLEY #58, TYLER CREEK MOBIL, HAMPSHIRE</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr"/>
+      <c r="H114" t="inlineStr"/>
+      <c r="I114" t="inlineStr"/>
+      <c r="J114" t="inlineStr"/>
+      <c r="K114" t="inlineStr"/>
+      <c r="L114" t="inlineStr"/>
+      <c r="M114" t="inlineStr"/>
+      <c r="N114" t="inlineStr"/>
+      <c r="O114" t="inlineStr"/>
+      <c r="P114" t="inlineStr"/>
+      <c r="Q114" t="inlineStr"/>
+      <c r="R114" t="inlineStr"/>
+      <c r="S114" t="inlineStr"/>
+      <c r="T114" t="inlineStr"/>
+      <c r="U114" t="inlineStr"/>
+      <c r="V114" t="inlineStr"/>
+      <c r="W114" t="inlineStr"/>
+      <c r="X114" t="inlineStr"/>
+      <c r="Y114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr"/>
+      <c r="B115" t="inlineStr"/>
+      <c r="C115" t="inlineStr"/>
+      <c r="D115" t="inlineStr"/>
+      <c r="E115" t="inlineStr"/>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>15N341 RTE 47</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr"/>
+      <c r="H115" t="inlineStr"/>
+      <c r="I115" t="inlineStr"/>
+      <c r="J115" t="inlineStr"/>
+      <c r="K115" t="inlineStr"/>
+      <c r="L115" t="inlineStr"/>
+      <c r="M115" t="inlineStr"/>
+      <c r="N115" t="inlineStr"/>
+      <c r="O115" t="inlineStr"/>
+      <c r="P115" t="inlineStr"/>
+      <c r="Q115" t="inlineStr"/>
+      <c r="R115" t="inlineStr"/>
+      <c r="S115" t="inlineStr"/>
+      <c r="T115" t="inlineStr"/>
+      <c r="U115" t="inlineStr"/>
+      <c r="V115" t="inlineStr"/>
+      <c r="W115" t="inlineStr"/>
+      <c r="X115" t="inlineStr"/>
+      <c r="Y115" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr"/>
+      <c r="B116" t="inlineStr"/>
+      <c r="C116" t="inlineStr"/>
+      <c r="D116" t="inlineStr"/>
+      <c r="E116" t="inlineStr"/>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/SW6S8XqhdGcLz6W2A</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr"/>
+      <c r="H116" t="inlineStr"/>
+      <c r="I116" t="inlineStr"/>
+      <c r="J116" t="inlineStr"/>
+      <c r="K116" t="inlineStr"/>
+      <c r="L116" t="inlineStr"/>
+      <c r="M116" t="inlineStr"/>
+      <c r="N116" t="inlineStr"/>
+      <c r="O116" t="inlineStr"/>
+      <c r="P116" t="inlineStr"/>
+      <c r="Q116" t="inlineStr"/>
+      <c r="R116" t="inlineStr"/>
+      <c r="S116" t="inlineStr"/>
+      <c r="T116" t="inlineStr"/>
+      <c r="U116" t="inlineStr"/>
+      <c r="V116" t="inlineStr"/>
+      <c r="W116" t="inlineStr"/>
+      <c r="X116" t="inlineStr"/>
+      <c r="Y116" t="inlineStr"/>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr"/>
+      <c r="B117" t="inlineStr"/>
+      <c r="C117" t="inlineStr"/>
+      <c r="D117" t="inlineStr"/>
+      <c r="E117" t="inlineStr"/>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>*IL Meet is 5:45 am at IL Office</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr"/>
+      <c r="H117" t="inlineStr"/>
+      <c r="I117" t="inlineStr"/>
+      <c r="J117" t="inlineStr"/>
+      <c r="K117" t="inlineStr"/>
+      <c r="L117" t="inlineStr"/>
+      <c r="M117" t="inlineStr"/>
+      <c r="N117" t="inlineStr"/>
+      <c r="O117" t="inlineStr"/>
+      <c r="P117" t="inlineStr"/>
+      <c r="Q117" t="inlineStr"/>
+      <c r="R117" t="inlineStr"/>
+      <c r="S117" t="inlineStr"/>
+      <c r="T117" t="inlineStr"/>
+      <c r="U117" t="inlineStr"/>
+      <c r="V117" t="inlineStr"/>
+      <c r="W117" t="inlineStr"/>
+      <c r="X117" t="inlineStr"/>
+      <c r="Y117" t="inlineStr"/>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr"/>
+      <c r="B118" t="inlineStr"/>
+      <c r="C118" t="inlineStr"/>
+      <c r="D118" t="inlineStr"/>
+      <c r="E118" t="inlineStr"/>
+      <c r="F118" t="inlineStr"/>
+      <c r="G118" t="inlineStr"/>
+      <c r="H118" t="inlineStr"/>
+      <c r="I118" t="inlineStr"/>
+      <c r="J118" t="inlineStr"/>
+      <c r="K118" t="inlineStr"/>
+      <c r="L118" t="inlineStr"/>
+      <c r="M118" t="inlineStr"/>
+      <c r="N118" t="inlineStr"/>
+      <c r="O118" t="inlineStr"/>
+      <c r="P118" t="inlineStr"/>
+      <c r="Q118" t="inlineStr"/>
+      <c r="R118" t="inlineStr"/>
+      <c r="S118" t="inlineStr"/>
+      <c r="T118" t="inlineStr"/>
+      <c r="U118" t="inlineStr"/>
+      <c r="V118" t="inlineStr"/>
+      <c r="W118" t="inlineStr"/>
+      <c r="X118" t="inlineStr"/>
+      <c r="Y118" t="inlineStr"/>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr"/>
+      <c r="B119" t="inlineStr"/>
+      <c r="C119" t="inlineStr"/>
+      <c r="D119" t="inlineStr"/>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Mike G</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>@ Store</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr"/>
+      <c r="I119" t="inlineStr"/>
+      <c r="J119" t="inlineStr"/>
+      <c r="K119" t="inlineStr"/>
+      <c r="L119" t="inlineStr"/>
+      <c r="M119" t="inlineStr"/>
+      <c r="N119" t="inlineStr"/>
+      <c r="O119" t="inlineStr"/>
+      <c r="P119" t="inlineStr"/>
+      <c r="Q119" t="inlineStr"/>
+      <c r="R119" t="inlineStr"/>
+      <c r="S119" t="inlineStr"/>
+      <c r="T119" t="inlineStr"/>
+      <c r="U119" t="inlineStr"/>
+      <c r="V119" t="inlineStr"/>
+      <c r="W119" t="inlineStr"/>
+      <c r="X119" t="inlineStr"/>
+      <c r="Y119" t="inlineStr"/>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr"/>
+      <c r="B120" t="inlineStr"/>
+      <c r="C120" t="inlineStr"/>
+      <c r="D120" t="inlineStr"/>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Angela</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr"/>
+      <c r="H120" t="inlineStr"/>
+      <c r="I120" t="inlineStr"/>
+      <c r="J120" t="inlineStr"/>
+      <c r="K120" t="inlineStr"/>
+      <c r="L120" t="inlineStr"/>
+      <c r="M120" t="inlineStr"/>
+      <c r="N120" t="inlineStr"/>
+      <c r="O120" t="inlineStr"/>
+      <c r="P120" t="inlineStr"/>
+      <c r="Q120" t="inlineStr"/>
+      <c r="R120" t="inlineStr"/>
+      <c r="S120" t="inlineStr"/>
+      <c r="T120" t="inlineStr"/>
+      <c r="U120" t="inlineStr"/>
+      <c r="V120" t="inlineStr"/>
+      <c r="W120" t="inlineStr"/>
+      <c r="X120" t="inlineStr"/>
+      <c r="Y120" t="inlineStr"/>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr"/>
+      <c r="B121" t="inlineStr"/>
+      <c r="C121" t="inlineStr"/>
+      <c r="D121" t="inlineStr"/>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>3)</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Emily L</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr"/>
+      <c r="H121" t="inlineStr"/>
+      <c r="I121" t="inlineStr"/>
+      <c r="J121" t="inlineStr"/>
+      <c r="K121" t="inlineStr"/>
+      <c r="L121" t="inlineStr"/>
+      <c r="M121" t="inlineStr"/>
+      <c r="N121" t="inlineStr"/>
+      <c r="O121" t="inlineStr"/>
+      <c r="P121" t="inlineStr"/>
+      <c r="Q121" t="inlineStr"/>
+      <c r="R121" t="inlineStr"/>
+      <c r="S121" t="inlineStr"/>
+      <c r="T121" t="inlineStr"/>
+      <c r="U121" t="inlineStr"/>
+      <c r="V121" t="inlineStr"/>
+      <c r="W121" t="inlineStr"/>
+      <c r="X121" t="inlineStr"/>
+      <c r="Y121" t="inlineStr"/>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr"/>
+      <c r="B122" t="inlineStr"/>
+      <c r="C122" t="inlineStr"/>
+      <c r="D122" t="inlineStr"/>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>4)</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Justin</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>Driver,
+Gray Van</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr"/>
+      <c r="I122" t="inlineStr"/>
+      <c r="J122" t="inlineStr"/>
+      <c r="K122" t="inlineStr"/>
+      <c r="L122" t="inlineStr"/>
+      <c r="M122" t="inlineStr"/>
+      <c r="N122" t="inlineStr"/>
+      <c r="O122" t="inlineStr"/>
+      <c r="P122" t="inlineStr"/>
+      <c r="Q122" t="inlineStr"/>
+      <c r="R122" t="inlineStr"/>
+      <c r="S122" t="inlineStr"/>
+      <c r="T122" t="inlineStr"/>
+      <c r="U122" t="inlineStr"/>
+      <c r="V122" t="inlineStr"/>
+      <c r="W122" t="inlineStr"/>
+      <c r="X122" t="inlineStr"/>
+      <c r="Y122" t="inlineStr"/>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr"/>
+      <c r="B123" t="inlineStr"/>
+      <c r="C123" t="inlineStr"/>
+      <c r="D123" t="inlineStr"/>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>5)</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>Krystin</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr"/>
+      <c r="H123" t="inlineStr"/>
+      <c r="I123" t="inlineStr"/>
+      <c r="J123" t="inlineStr"/>
+      <c r="K123" t="inlineStr"/>
+      <c r="L123" t="inlineStr"/>
+      <c r="M123" t="inlineStr"/>
+      <c r="N123" t="inlineStr"/>
+      <c r="O123" t="inlineStr"/>
+      <c r="P123" t="inlineStr"/>
+      <c r="Q123" t="inlineStr"/>
+      <c r="R123" t="inlineStr"/>
+      <c r="S123" t="inlineStr"/>
+      <c r="T123" t="inlineStr"/>
+      <c r="U123" t="inlineStr"/>
+      <c r="V123" t="inlineStr"/>
+      <c r="W123" t="inlineStr"/>
+      <c r="X123" t="inlineStr"/>
+      <c r="Y123" t="inlineStr"/>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr"/>
+      <c r="B124" t="inlineStr"/>
+      <c r="C124" t="inlineStr"/>
+      <c r="D124" t="inlineStr"/>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>6)</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>Taylor</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr"/>
+      <c r="H124" t="inlineStr"/>
+      <c r="I124" t="inlineStr"/>
+      <c r="J124" t="inlineStr"/>
+      <c r="K124" t="inlineStr"/>
+      <c r="L124" t="inlineStr"/>
+      <c r="M124" t="inlineStr"/>
+      <c r="N124" t="inlineStr"/>
+      <c r="O124" t="inlineStr"/>
+      <c r="P124" t="inlineStr"/>
+      <c r="Q124" t="inlineStr"/>
+      <c r="R124" t="inlineStr"/>
+      <c r="S124" t="inlineStr"/>
+      <c r="T124" t="inlineStr"/>
+      <c r="U124" t="inlineStr"/>
+      <c r="V124" t="inlineStr"/>
+      <c r="W124" t="inlineStr"/>
+      <c r="X124" t="inlineStr"/>
+      <c r="Y124" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>